<commit_message>
task 2 code and figures, and update the excel file with the new wind scenarios.
</commit_message>
<xml_diff>
--- a/A2/ieee9-wind.xlsx
+++ b/A2/ieee9-wind.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5ef074c61d2afe73/Desktop/Stefano/In_the_NL/TAing and FlexDelft/SET3065 TAing/Assignments/Assignments/A2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\doron\Documents\TU Delft\Q3\IEPG SET3065\Assignments-SET3065-2026\IEPG-SET3065\A2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{4450768D-02F8-4D1C-8527-7C7DEAF1A662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0964318-C399-49FD-B7D0-244EC48146D1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FD8C0C-11DB-4BD6-97B3-9EEA2DFB71E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -1017,9 +1017,9 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1076,9 +1076,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>73</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>75</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>76</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>77</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>78</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>79</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>82</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>83</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>87</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>89</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>90</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>91</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>3.9300000000000003E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>93</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>94</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>95</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>96</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>97</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>98</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>99</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>100</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>101</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>102</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>103</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>104</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>105</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>107</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>108</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>109</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>110</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>111</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>114</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>116</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>117</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>118</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>119</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>120</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>121</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>122</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>4.0299999999999997E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>123</v>
       </c>
@@ -2438,9 +2438,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>127</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>128</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>129</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>130</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>131</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>133</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>134</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>135</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>136</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>137</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>138</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>139</v>
       </c>
@@ -3243,9 +3243,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>144</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -3466,9 +3466,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>1.7594151723123451E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>9.6953812481870865E-8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>5.733508454939855E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3580,7 +3580,7 @@
         <v>3.5594094351783463E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>9.1265899103041392E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>6.6769026345706278E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>0.21098629100401939</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>9.1263139543015945E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>0.1472939750805019</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>0.3117069393387471</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>0.38417345908056261</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3775,9 +3775,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>161</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3868,7 +3868,7 @@
         <v>7.7265523480447653</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>53.771577418010231</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3962,7 +3962,7 @@
         <v>35.167509104339132</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4009,7 +4009,7 @@
         <v>19.837731862674321</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>39.835177967390138</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>18.27193181523721</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4161,9 +4161,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>175</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>16.20588096429206</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4292,7 +4292,7 @@
         <v>14.43901142858452</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>25.29573231860725</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4380,7 +4380,7 @@
         <v>88.800496098066986</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4435,9 +4435,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4467,9 +4467,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4499,7 +4499,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4521,9 +4521,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>1.0499984526720501</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>1.049998736379713</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4599,9 +4599,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4626,7 +4626,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -4640,7 +4640,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -4668,7 +4668,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -4752,7 +4752,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4808,7 +4808,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4836,7 +4836,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4892,7 +4892,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4920,7 +4920,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4948,7 +4948,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4976,7 +4976,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4990,7 +4990,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -5102,7 +5102,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -5116,7 +5116,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -5158,7 +5158,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -5214,7 +5214,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -5270,7 +5270,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5466,7 +5466,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5522,7 +5522,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5578,7 +5578,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5620,7 +5620,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5676,7 +5676,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5690,7 +5690,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5732,7 +5732,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5788,7 +5788,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5802,7 +5802,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5830,7 +5830,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5858,7 +5858,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6012,7 +6012,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6096,7 +6096,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6124,7 +6124,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6180,7 +6180,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -6222,7 +6222,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -6236,7 +6236,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -6264,7 +6264,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -6292,7 +6292,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -6306,7 +6306,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -6348,7 +6348,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -6376,7 +6376,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -6404,7 +6404,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -6431,14 +6431,14 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -6591,7 +6591,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6617,7 +6617,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6786,14 +6786,14 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -6860,7 +6860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6892,7 +6892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6937,9 +6937,9 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7072,17 +7072,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7169,9 +7169,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7240,9 +7240,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -7607,20 +7607,20 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -7744,7 +7744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -7844,12 +7844,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -7906,7 +7906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -7981,9 +7981,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>61</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -8096,7 +8096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -8131,6 +8131,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d7183f91-9bc1-4815-a8cc-657456d3f3e2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF69BC8263728E439106B51AAE1F9555" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4c1e435d715365c5c2eb4975be48707">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe" xmlns:ns3="d7183f91-9bc1-4815-a8cc-657456d3f3e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="019a01aa2e8d58df36c0a5bb35ed35f1" ns2:_="" ns3:_="">
     <xsd:import namespace="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe"/>
@@ -8325,34 +8345,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d7183f91-9bc1-4815-a8cc-657456d3f3e2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFCF7C6F-4A9E-49D1-9637-B693696D2528}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC2B5E33-2115-4068-8246-E3ABF935B199}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe"/>
+    <ds:schemaRef ds:uri="d7183f91-9bc1-4815-a8cc-657456d3f3e2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C97EB115-024D-49F6-8653-86B4C8A5F291}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C97EB115-024D-49F6-8653-86B4C8A5F291}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC2B5E33-2115-4068-8246-E3ABF935B199}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFCF7C6F-4A9E-49D1-9637-B693696D2528}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="12bfa3c6-642b-43fc-a2fb-3892ae41b4fe"/>
+    <ds:schemaRef ds:uri="d7183f91-9bc1-4815-a8cc-657456d3f3e2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>